<commit_message>
Feat(docs): new docs updated - 2026-01-26 22:57:22
</commit_message>
<xml_diff>
--- a/resultados_seace/01.26.2026-T2MDC.xlsx
+++ b/resultados_seace/01.26.2026-T2MDC.xlsx
@@ -534,7 +534,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>26/01/2026 22:17:55</t>
+          <t>26/01/2026 22:57:21</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -584,7 +584,11 @@
           <t>CONTRATACIÓN DEL SERVICIO DE CONFECCION E INSTALACION DE ESTRUCTURAS METALICAS Y COBERTURA PARA TECHO SEGÚN DISEÑO (A TODO COSTO) PARA EL PROYECTO ¿MEJORAMIENTO DEL SERVICIO DE PRÁCTICA DEPORTIVA Y/O RECREATIVA EN LA LOSA DEPORTIVA PAMPATAMA DISTRITO DE TINTAY DE LA PROVINCIA DE AYMARAES DEL DEPARTAMENTO DE APURIMAC¿ CUI - 2709576</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -592,7 +596,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>26/01/2026 22:17:55</t>
+          <t>26/01/2026 22:57:21</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -644,7 +648,7 @@
       </c>
       <c r="N3" s="2" t="inlineStr">
         <is>
-          <t>Ver .PDF</t>
+          <t>Ver Documento</t>
         </is>
       </c>
     </row>
@@ -654,7 +658,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>26/01/2026 22:17:55</t>
+          <t>26/01/2026 22:57:21</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -706,7 +710,7 @@
       </c>
       <c r="N4" s="2" t="inlineStr">
         <is>
-          <t>Ver .PDF</t>
+          <t>Ver Documento</t>
         </is>
       </c>
     </row>
@@ -716,7 +720,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>26/01/2026 22:17:55</t>
+          <t>26/01/2026 22:57:21</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -768,7 +772,7 @@
       </c>
       <c r="N5" s="2" t="inlineStr">
         <is>
-          <t>Ver .PDF</t>
+          <t>Ver Documento</t>
         </is>
       </c>
     </row>
@@ -778,7 +782,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>26/01/2026 22:17:55</t>
+          <t>26/01/2026 22:57:21</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -830,7 +834,7 @@
       </c>
       <c r="N6" s="2" t="inlineStr">
         <is>
-          <t>Ver .PDF</t>
+          <t>Ver Documento</t>
         </is>
       </c>
     </row>
@@ -840,7 +844,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26/01/2026 22:17:55</t>
+          <t>26/01/2026 22:57:21</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -892,7 +896,7 @@
       </c>
       <c r="N7" s="2" t="inlineStr">
         <is>
-          <t>Ver .PDF</t>
+          <t>Ver Documento</t>
         </is>
       </c>
     </row>
@@ -902,7 +906,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>26/01/2026 22:17:55</t>
+          <t>26/01/2026 22:57:21</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -954,18 +958,19 @@
       </c>
       <c r="N8" s="2" t="inlineStr">
         <is>
-          <t>Ver .PDF</t>
+          <t>Ver Documento</t>
         </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N3" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N4" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N5" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N6" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N7" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N8" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Feat(docs): new docs updated - 2026-01-26 23:28:57
</commit_message>
<xml_diff>
--- a/resultados_seace/01.26.2026-T2MDC.xlsx
+++ b/resultados_seace/01.26.2026-T2MDC.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,7 +534,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>26/01/2026 22:57:21</t>
+          <t>26/01/2026 23:28:57</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -596,22 +596,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>26/01/2026 22:57:21</t>
+          <t>26/01/2026 23:28:57</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>26/01/2026 19:11</t>
+          <t>26/01/2026 20:38</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CP-ABR-2-2026-MPS-C-1</t>
+          <t>CP-ABR-1-2026-MDT-1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+          <t>MUNICIPALIDAD DISTRITAL DE TINTAY</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -643,7 +643,7 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>SERVCIO: "MANTENIMIENTO DEL DREN DOS DE MAYO ENTRE LA AV. PERU Y LA CALLE ELIAS VALLEJOS DEL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA, DEPARTAMENTO DE ANCASH"</t>
+          <t>CONTRATACIÓN DEL SERVICIO DE CONFECCION E INSTALACION DE ESTRUCTURAS METALICAS Y COBERTURA PARA TECHO SEGÚN DISEÑO (A TODO COSTO) PARA EL PROYECTO ¿MEJORAMIENTO DEL SERVICIO DE PRÁCTICA DEPORTIVA Y/O RECREATIVA EN LA LOSA DEPORTIVA PAMPATAMA DISTRITO DE TINTAY DE LA PROVINCIA DE AYMARAES DEL DEPARTAMENTO DE APURIMAC¿ CUI - 2709576</t>
         </is>
       </c>
       <c r="N3" s="2" t="inlineStr">
@@ -658,22 +658,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>26/01/2026 22:57:21</t>
+          <t>26/01/2026 23:28:57</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>26/01/2026 18:57</t>
+          <t>26/01/2026 20:38</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CP-ABR-1-2026-MPS-C-1</t>
+          <t>CP-ABR-1-2026-MDT-1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+          <t>MUNICIPALIDAD DISTRITAL DE TINTAY</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -705,7 +705,7 @@
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>SERVICIO: "MANTENIMIENTO DEL AUDITORIO DEL PALACIO MUNICIPAL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA - ANCASH".</t>
+          <t>CONTRATACIÓN DEL SERVICIO DE CONFECCION E INSTALACION DE ESTRUCTURAS METALICAS Y COBERTURA PARA TECHO SEGÚN DISEÑO (A TODO COSTO) PARA EL PROYECTO ¿MEJORAMIENTO DEL SERVICIO DE PRÁCTICA DEPORTIVA Y/O RECREATIVA EN LA LOSA DEPORTIVA PAMPATAMA DISTRITO DE TINTAY DE LA PROVINCIA DE AYMARAES DEL DEPARTAMENTO DE APURIMAC¿ CUI - 2709576</t>
         </is>
       </c>
       <c r="N4" s="2" t="inlineStr">
@@ -720,22 +720,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>26/01/2026 22:57:21</t>
+          <t>26/01/2026 23:28:57</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>26/01/2026 18:37</t>
+          <t>26/01/2026 20:38</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CP-ABR-1-2026-PNSR-1</t>
+          <t>CP-ABR-1-2026-MDT-1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+          <t>MUNICIPALIDAD DISTRITAL DE TINTAY</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -767,7 +767,7 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>SERVICIO DE SEGUROS PATRIMONIALES Y VEHICULARES DEL PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+          <t>CONTRATACIÓN DEL SERVICIO DE CONFECCION E INSTALACION DE ESTRUCTURAS METALICAS Y COBERTURA PARA TECHO SEGÚN DISEÑO (A TODO COSTO) PARA EL PROYECTO ¿MEJORAMIENTO DEL SERVICIO DE PRÁCTICA DEPORTIVA Y/O RECREATIVA EN LA LOSA DEPORTIVA PAMPATAMA DISTRITO DE TINTAY DE LA PROVINCIA DE AYMARAES DEL DEPARTAMENTO DE APURIMAC¿ CUI - 2709576</t>
         </is>
       </c>
       <c r="N5" s="2" t="inlineStr">
@@ -782,22 +782,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>26/01/2026 22:57:21</t>
+          <t>26/01/2026 23:28:57</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>26/01/2026 15:28</t>
+          <t>26/01/2026 20:38</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CP-ABR-13-2025-MPA/C-2</t>
+          <t>CP-ABR-1-2026-MDT-1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>MUNICIPALIDAD PROVINCIAL DE AREQUIPA</t>
+          <t>MUNICIPALIDAD DISTRITAL DE TINTAY</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>04/02/2026 23:59</t>
+          <t>03/02/2026 23:59</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -823,13 +823,13 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>05/02/2026 23:59</t>
+          <t>04/02/2026 23:59</t>
         </is>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>SERVICIO DE CONSULTORÍA PARA LA ELABORACIÓN DE UN PLAN DE SOSTENIBILIDAD URBANO - AMBIENTAL PARA LA REVITALIZACIÓN URBANA DE LA MACRO MANZANA DEL MERCADO SAN CAMILO EN EL CENTRO HISTÓRICO DE AREQUIPA, DISTRITO DE AREQUIPA PROVINCIA DE AREQUIPA, DEPARTAMENTO DE AREQUIPA; PARA LA GERENCIA DE CENTRO HI</t>
+          <t>CONTRATACIÓN DEL SERVICIO DE CONFECCION E INSTALACION DE ESTRUCTURAS METALICAS Y COBERTURA PARA TECHO SEGÚN DISEÑO (A TODO COSTO) PARA EL PROYECTO ¿MEJORAMIENTO DEL SERVICIO DE PRÁCTICA DEPORTIVA Y/O RECREATIVA EN LA LOSA DEPORTIVA PAMPATAMA DISTRITO DE TINTAY DE LA PROVINCIA DE AYMARAES DEL DEPARTAMENTO DE APURIMAC¿ CUI - 2709576</t>
         </is>
       </c>
       <c r="N6" s="2" t="inlineStr">
@@ -844,22 +844,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26/01/2026 22:57:21</t>
+          <t>26/01/2026 23:28:57</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>26/01/2026 15:03</t>
+          <t>26/01/2026 20:38</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CP SER-SM-1-2026-MPCH-OC-1</t>
+          <t>CP-ABR-1-2026-MDT-1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>MUNICIPALIDAD PROVINCIAL DE CHINCHA - CHINCHA ALTA</t>
+          <t>MUNICIPALIDAD DISTRITAL DE TINTAY</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -869,29 +869,29 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>24/02/2026 23:59</t>
+          <t>03/02/2026 23:59</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>04/02/2026 23:59</t>
+          <t>29/01/2026 23:59</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>09/02/2026</t>
+          <t>30/01/2026</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>25/02/2026 23:59</t>
+          <t>04/02/2026 23:59</t>
         </is>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>SERVICIO: MANTENIMIENTO DEL SERVICIO DE TRANSITABILIDAD VEHICULAR Y PEATONAL EN LAS CALLES MOISES FLORES, ANDRES RAZURI, ARICA, MARISCAL CASTILLA, AV. FAUSTINO SANCHEZ CARRIÓN Y AV. TUPAC AMARU DEL DISTRITO DE CHINCHA ALTA PROVINCIA DE CHINCHA DEPARTAMENTO DE ICA</t>
+          <t>CONTRATACIÓN DEL SERVICIO DE CONFECCION E INSTALACION DE ESTRUCTURAS METALICAS Y COBERTURA PARA TECHO SEGÚN DISEÑO (A TODO COSTO) PARA EL PROYECTO ¿MEJORAMIENTO DEL SERVICIO DE PRÁCTICA DEPORTIVA Y/O RECREATIVA EN LA LOSA DEPORTIVA PAMPATAMA DISTRITO DE TINTAY DE LA PROVINCIA DE AYMARAES DEL DEPARTAMENTO DE APURIMAC¿ CUI - 2709576</t>
         </is>
       </c>
       <c r="N7" s="2" t="inlineStr">
@@ -906,22 +906,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>26/01/2026 22:57:21</t>
+          <t>26/01/2026 23:28:57</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>26/01/2026 13:00</t>
+          <t>26/01/2026 20:38</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CP-ABR-6-2026-ESSALUD/RATU-2</t>
+          <t>CP-ABR-1-2026-MDT-1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>SEGURO SOCIAL DE SALUD</t>
+          <t>MUNICIPALIDAD DISTRITAL DE TINTAY</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -953,10 +953,3482 @@
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr">
         <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE CONFECCION E INSTALACION DE ESTRUCTURAS METALICAS Y COBERTURA PARA TECHO SEGÚN DISEÑO (A TODO COSTO) PARA EL PROYECTO ¿MEJORAMIENTO DEL SERVICIO DE PRÁCTICA DEPORTIVA Y/O RECREATIVA EN LA LOSA DEPORTIVA PAMPATAMA DISTRITO DE TINTAY DE LA PROVINCIA DE AYMARAES DEL DEPARTAMENTO DE APURIMAC¿ CUI - 2709576</t>
+        </is>
+      </c>
+      <c r="N8" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>26/01/2026 20:38</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MDT-1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD DISTRITAL DE TINTAY</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE CONFECCION E INSTALACION DE ESTRUCTURAS METALICAS Y COBERTURA PARA TECHO SEGÚN DISEÑO (A TODO COSTO) PARA EL PROYECTO ¿MEJORAMIENTO DEL SERVICIO DE PRÁCTICA DEPORTIVA Y/O RECREATIVA EN LA LOSA DEPORTIVA PAMPATAMA DISTRITO DE TINTAY DE LA PROVINCIA DE AYMARAES DEL DEPARTAMENTO DE APURIMAC¿ CUI - 2709576</t>
+        </is>
+      </c>
+      <c r="N9" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>26/01/2026 20:38</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MDT-1</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD DISTRITAL DE TINTAY</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE CONFECCION E INSTALACION DE ESTRUCTURAS METALICAS Y COBERTURA PARA TECHO SEGÚN DISEÑO (A TODO COSTO) PARA EL PROYECTO ¿MEJORAMIENTO DEL SERVICIO DE PRÁCTICA DEPORTIVA Y/O RECREATIVA EN LA LOSA DEPORTIVA PAMPATAMA DISTRITO DE TINTAY DE LA PROVINCIA DE AYMARAES DEL DEPARTAMENTO DE APURIMAC¿ CUI - 2709576</t>
+        </is>
+      </c>
+      <c r="N10" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>26/01/2026 19:11</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>CP-ABR-2-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>SERVCIO: "MANTENIMIENTO DEL DREN DOS DE MAYO ENTRE LA AV. PERU Y LA CALLE ELIAS VALLEJOS DEL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA, DEPARTAMENTO DE ANCASH"</t>
+        </is>
+      </c>
+      <c r="N11" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>26/01/2026 19:11</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>CP-ABR-2-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>SERVCIO: "MANTENIMIENTO DEL DREN DOS DE MAYO ENTRE LA AV. PERU Y LA CALLE ELIAS VALLEJOS DEL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA, DEPARTAMENTO DE ANCASH"</t>
+        </is>
+      </c>
+      <c r="N12" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>26/01/2026 19:11</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>CP-ABR-2-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>SERVCIO: "MANTENIMIENTO DEL DREN DOS DE MAYO ENTRE LA AV. PERU Y LA CALLE ELIAS VALLEJOS DEL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA, DEPARTAMENTO DE ANCASH"</t>
+        </is>
+      </c>
+      <c r="N13" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>26/01/2026 19:11</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>CP-ABR-2-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>SERVCIO: "MANTENIMIENTO DEL DREN DOS DE MAYO ENTRE LA AV. PERU Y LA CALLE ELIAS VALLEJOS DEL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA, DEPARTAMENTO DE ANCASH"</t>
+        </is>
+      </c>
+      <c r="N14" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>26/01/2026 19:11</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>CP-ABR-2-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>SERVCIO: "MANTENIMIENTO DEL DREN DOS DE MAYO ENTRE LA AV. PERU Y LA CALLE ELIAS VALLEJOS DEL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA, DEPARTAMENTO DE ANCASH"</t>
+        </is>
+      </c>
+      <c r="N15" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>26/01/2026 19:11</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>CP-ABR-2-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>SERVCIO: "MANTENIMIENTO DEL DREN DOS DE MAYO ENTRE LA AV. PERU Y LA CALLE ELIAS VALLEJOS DEL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA, DEPARTAMENTO DE ANCASH"</t>
+        </is>
+      </c>
+      <c r="N16" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>26/01/2026 19:11</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>CP-ABR-2-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>SERVCIO: "MANTENIMIENTO DEL DREN DOS DE MAYO ENTRE LA AV. PERU Y LA CALLE ELIAS VALLEJOS DEL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA, DEPARTAMENTO DE ANCASH"</t>
+        </is>
+      </c>
+      <c r="N17" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>26/01/2026 19:11</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CP-ABR-2-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>SERVCIO: "MANTENIMIENTO DEL DREN DOS DE MAYO ENTRE LA AV. PERU Y LA CALLE ELIAS VALLEJOS DEL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA, DEPARTAMENTO DE ANCASH"</t>
+        </is>
+      </c>
+      <c r="N18" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>26/01/2026 19:11</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>CP-ABR-2-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>SERVCIO: "MANTENIMIENTO DEL DREN DOS DE MAYO ENTRE LA AV. PERU Y LA CALLE ELIAS VALLEJOS DEL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA, DEPARTAMENTO DE ANCASH"</t>
+        </is>
+      </c>
+      <c r="N19" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:57</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>SERVICIO: "MANTENIMIENTO DEL AUDITORIO DEL PALACIO MUNICIPAL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA - ANCASH".</t>
+        </is>
+      </c>
+      <c r="N20" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:57</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>SERVICIO: "MANTENIMIENTO DEL AUDITORIO DEL PALACIO MUNICIPAL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA - ANCASH".</t>
+        </is>
+      </c>
+      <c r="N21" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:57</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>SERVICIO: "MANTENIMIENTO DEL AUDITORIO DEL PALACIO MUNICIPAL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA - ANCASH".</t>
+        </is>
+      </c>
+      <c r="N22" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:57</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>SERVICIO: "MANTENIMIENTO DEL AUDITORIO DEL PALACIO MUNICIPAL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA - ANCASH".</t>
+        </is>
+      </c>
+      <c r="N23" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:57</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>SERVICIO: "MANTENIMIENTO DEL AUDITORIO DEL PALACIO MUNICIPAL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA - ANCASH".</t>
+        </is>
+      </c>
+      <c r="N24" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:57</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>SERVICIO: "MANTENIMIENTO DEL AUDITORIO DEL PALACIO MUNICIPAL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA - ANCASH".</t>
+        </is>
+      </c>
+      <c r="N25" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:57</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>SERVICIO: "MANTENIMIENTO DEL AUDITORIO DEL PALACIO MUNICIPAL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA - ANCASH".</t>
+        </is>
+      </c>
+      <c r="N26" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:57</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>SERVICIO: "MANTENIMIENTO DEL AUDITORIO DEL PALACIO MUNICIPAL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA - ANCASH".</t>
+        </is>
+      </c>
+      <c r="N27" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:57</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-MPS-C-1</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE SANTA - CHIMBOTE</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>SERVICIO: "MANTENIMIENTO DEL AUDITORIO DEL PALACIO MUNICIPAL DISTRITO DE CHIMBOTE, PROVINCIA DEL SANTA - ANCASH".</t>
+        </is>
+      </c>
+      <c r="N28" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:37</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-PNSR-1</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>SERVICIO DE SEGUROS PATRIMONIALES Y VEHICULARES DEL PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="N29" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:37</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-PNSR-1</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>SERVICIO DE SEGUROS PATRIMONIALES Y VEHICULARES DEL PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="N30" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:37</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-PNSR-1</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>SERVICIO DE SEGUROS PATRIMONIALES Y VEHICULARES DEL PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="N31" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:37</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-PNSR-1</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>SERVICIO DE SEGUROS PATRIMONIALES Y VEHICULARES DEL PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="N32" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:37</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-PNSR-1</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>SERVICIO DE SEGUROS PATRIMONIALES Y VEHICULARES DEL PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="N33" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:37</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-PNSR-1</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>SERVICIO DE SEGUROS PATRIMONIALES Y VEHICULARES DEL PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="N34" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:37</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-PNSR-1</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>SERVICIO DE SEGUROS PATRIMONIALES Y VEHICULARES DEL PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="N35" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:37</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-PNSR-1</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>SERVICIO DE SEGUROS PATRIMONIALES Y VEHICULARES DEL PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="N36" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>26/01/2026 18:37</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>CP-ABR-1-2026-PNSR-1</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>SERVICIO DE SEGUROS PATRIMONIALES Y VEHICULARES DEL PROGRAMA NACIONAL DE SANEAMIENTO RURAL</t>
+        </is>
+      </c>
+      <c r="N37" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:28</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>CP-ABR-13-2025-MPA/C-2</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE AREQUIPA</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>05/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>SERVICIO DE CONSULTORÍA PARA LA ELABORACIÓN DE UN PLAN DE SOSTENIBILIDAD URBANO - AMBIENTAL PARA LA REVITALIZACIÓN URBANA DE LA MACRO MANZANA DEL MERCADO SAN CAMILO EN EL CENTRO HISTÓRICO DE AREQUIPA, DISTRITO DE AREQUIPA PROVINCIA DE AREQUIPA, DEPARTAMENTO DE AREQUIPA; PARA LA GERENCIA DE CENTRO HI</t>
+        </is>
+      </c>
+      <c r="N38" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:28</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>CP-ABR-13-2025-MPA/C-2</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE AREQUIPA</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>05/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>SERVICIO DE CONSULTORÍA PARA LA ELABORACIÓN DE UN PLAN DE SOSTENIBILIDAD URBANO - AMBIENTAL PARA LA REVITALIZACIÓN URBANA DE LA MACRO MANZANA DEL MERCADO SAN CAMILO EN EL CENTRO HISTÓRICO DE AREQUIPA, DISTRITO DE AREQUIPA PROVINCIA DE AREQUIPA, DEPARTAMENTO DE AREQUIPA; PARA LA GERENCIA DE CENTRO HI</t>
+        </is>
+      </c>
+      <c r="N39" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:28</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>CP-ABR-13-2025-MPA/C-2</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE AREQUIPA</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>05/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>SERVICIO DE CONSULTORÍA PARA LA ELABORACIÓN DE UN PLAN DE SOSTENIBILIDAD URBANO - AMBIENTAL PARA LA REVITALIZACIÓN URBANA DE LA MACRO MANZANA DEL MERCADO SAN CAMILO EN EL CENTRO HISTÓRICO DE AREQUIPA, DISTRITO DE AREQUIPA PROVINCIA DE AREQUIPA, DEPARTAMENTO DE AREQUIPA; PARA LA GERENCIA DE CENTRO HI</t>
+        </is>
+      </c>
+      <c r="N40" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:28</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>CP-ABR-13-2025-MPA/C-2</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE AREQUIPA</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>05/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>SERVICIO DE CONSULTORÍA PARA LA ELABORACIÓN DE UN PLAN DE SOSTENIBILIDAD URBANO - AMBIENTAL PARA LA REVITALIZACIÓN URBANA DE LA MACRO MANZANA DEL MERCADO SAN CAMILO EN EL CENTRO HISTÓRICO DE AREQUIPA, DISTRITO DE AREQUIPA PROVINCIA DE AREQUIPA, DEPARTAMENTO DE AREQUIPA; PARA LA GERENCIA DE CENTRO HI</t>
+        </is>
+      </c>
+      <c r="N41" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:28</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>CP-ABR-13-2025-MPA/C-2</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE AREQUIPA</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>05/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>SERVICIO DE CONSULTORÍA PARA LA ELABORACIÓN DE UN PLAN DE SOSTENIBILIDAD URBANO - AMBIENTAL PARA LA REVITALIZACIÓN URBANA DE LA MACRO MANZANA DEL MERCADO SAN CAMILO EN EL CENTRO HISTÓRICO DE AREQUIPA, DISTRITO DE AREQUIPA PROVINCIA DE AREQUIPA, DEPARTAMENTO DE AREQUIPA; PARA LA GERENCIA DE CENTRO HI</t>
+        </is>
+      </c>
+      <c r="N42" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:28</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>CP-ABR-13-2025-MPA/C-2</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE AREQUIPA</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>05/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>SERVICIO DE CONSULTORÍA PARA LA ELABORACIÓN DE UN PLAN DE SOSTENIBILIDAD URBANO - AMBIENTAL PARA LA REVITALIZACIÓN URBANA DE LA MACRO MANZANA DEL MERCADO SAN CAMILO EN EL CENTRO HISTÓRICO DE AREQUIPA, DISTRITO DE AREQUIPA PROVINCIA DE AREQUIPA, DEPARTAMENTO DE AREQUIPA; PARA LA GERENCIA DE CENTRO HI</t>
+        </is>
+      </c>
+      <c r="N43" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:28</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>CP-ABR-13-2025-MPA/C-2</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE AREQUIPA</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>05/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>SERVICIO DE CONSULTORÍA PARA LA ELABORACIÓN DE UN PLAN DE SOSTENIBILIDAD URBANO - AMBIENTAL PARA LA REVITALIZACIÓN URBANA DE LA MACRO MANZANA DEL MERCADO SAN CAMILO EN EL CENTRO HISTÓRICO DE AREQUIPA, DISTRITO DE AREQUIPA PROVINCIA DE AREQUIPA, DEPARTAMENTO DE AREQUIPA; PARA LA GERENCIA DE CENTRO HI</t>
+        </is>
+      </c>
+      <c r="N44" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:28</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>CP-ABR-13-2025-MPA/C-2</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE AREQUIPA</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>05/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>SERVICIO DE CONSULTORÍA PARA LA ELABORACIÓN DE UN PLAN DE SOSTENIBILIDAD URBANO - AMBIENTAL PARA LA REVITALIZACIÓN URBANA DE LA MACRO MANZANA DEL MERCADO SAN CAMILO EN EL CENTRO HISTÓRICO DE AREQUIPA, DISTRITO DE AREQUIPA PROVINCIA DE AREQUIPA, DEPARTAMENTO DE AREQUIPA; PARA LA GERENCIA DE CENTRO HI</t>
+        </is>
+      </c>
+      <c r="N45" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:28</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>CP-ABR-13-2025-MPA/C-2</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE AREQUIPA</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>05/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>SERVICIO DE CONSULTORÍA PARA LA ELABORACIÓN DE UN PLAN DE SOSTENIBILIDAD URBANO - AMBIENTAL PARA LA REVITALIZACIÓN URBANA DE LA MACRO MANZANA DEL MERCADO SAN CAMILO EN EL CENTRO HISTÓRICO DE AREQUIPA, DISTRITO DE AREQUIPA PROVINCIA DE AREQUIPA, DEPARTAMENTO DE AREQUIPA; PARA LA GERENCIA DE CENTRO HI</t>
+        </is>
+      </c>
+      <c r="N46" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:03</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>CP SER-SM-1-2026-MPCH-OC-1</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE CHINCHA - CHINCHA ALTA</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>24/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>09/02/2026</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>25/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>SERVICIO: MANTENIMIENTO DEL SERVICIO DE TRANSITABILIDAD VEHICULAR Y PEATONAL EN LAS CALLES MOISES FLORES, ANDRES RAZURI, ARICA, MARISCAL CASTILLA, AV. FAUSTINO SANCHEZ CARRIÓN Y AV. TUPAC AMARU DEL DISTRITO DE CHINCHA ALTA PROVINCIA DE CHINCHA DEPARTAMENTO DE ICA</t>
+        </is>
+      </c>
+      <c r="N47" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:03</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>CP SER-SM-1-2026-MPCH-OC-1</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE CHINCHA - CHINCHA ALTA</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>24/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>09/02/2026</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>25/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>SERVICIO: MANTENIMIENTO DEL SERVICIO DE TRANSITABILIDAD VEHICULAR Y PEATONAL EN LAS CALLES MOISES FLORES, ANDRES RAZURI, ARICA, MARISCAL CASTILLA, AV. FAUSTINO SANCHEZ CARRIÓN Y AV. TUPAC AMARU DEL DISTRITO DE CHINCHA ALTA PROVINCIA DE CHINCHA DEPARTAMENTO DE ICA</t>
+        </is>
+      </c>
+      <c r="N48" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:03</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>CP SER-SM-1-2026-MPCH-OC-1</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE CHINCHA - CHINCHA ALTA</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>24/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>09/02/2026</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>25/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>SERVICIO: MANTENIMIENTO DEL SERVICIO DE TRANSITABILIDAD VEHICULAR Y PEATONAL EN LAS CALLES MOISES FLORES, ANDRES RAZURI, ARICA, MARISCAL CASTILLA, AV. FAUSTINO SANCHEZ CARRIÓN Y AV. TUPAC AMARU DEL DISTRITO DE CHINCHA ALTA PROVINCIA DE CHINCHA DEPARTAMENTO DE ICA</t>
+        </is>
+      </c>
+      <c r="N49" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:03</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>CP SER-SM-1-2026-MPCH-OC-1</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE CHINCHA - CHINCHA ALTA</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>24/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>09/02/2026</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>25/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>SERVICIO: MANTENIMIENTO DEL SERVICIO DE TRANSITABILIDAD VEHICULAR Y PEATONAL EN LAS CALLES MOISES FLORES, ANDRES RAZURI, ARICA, MARISCAL CASTILLA, AV. FAUSTINO SANCHEZ CARRIÓN Y AV. TUPAC AMARU DEL DISTRITO DE CHINCHA ALTA PROVINCIA DE CHINCHA DEPARTAMENTO DE ICA</t>
+        </is>
+      </c>
+      <c r="N50" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:03</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>CP SER-SM-1-2026-MPCH-OC-1</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE CHINCHA - CHINCHA ALTA</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>24/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>09/02/2026</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>25/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>SERVICIO: MANTENIMIENTO DEL SERVICIO DE TRANSITABILIDAD VEHICULAR Y PEATONAL EN LAS CALLES MOISES FLORES, ANDRES RAZURI, ARICA, MARISCAL CASTILLA, AV. FAUSTINO SANCHEZ CARRIÓN Y AV. TUPAC AMARU DEL DISTRITO DE CHINCHA ALTA PROVINCIA DE CHINCHA DEPARTAMENTO DE ICA</t>
+        </is>
+      </c>
+      <c r="N51" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:03</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>CP SER-SM-1-2026-MPCH-OC-1</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE CHINCHA - CHINCHA ALTA</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>24/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>09/02/2026</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>25/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>SERVICIO: MANTENIMIENTO DEL SERVICIO DE TRANSITABILIDAD VEHICULAR Y PEATONAL EN LAS CALLES MOISES FLORES, ANDRES RAZURI, ARICA, MARISCAL CASTILLA, AV. FAUSTINO SANCHEZ CARRIÓN Y AV. TUPAC AMARU DEL DISTRITO DE CHINCHA ALTA PROVINCIA DE CHINCHA DEPARTAMENTO DE ICA</t>
+        </is>
+      </c>
+      <c r="N52" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:03</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>CP SER-SM-1-2026-MPCH-OC-1</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE CHINCHA - CHINCHA ALTA</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>24/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>09/02/2026</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>25/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>SERVICIO: MANTENIMIENTO DEL SERVICIO DE TRANSITABILIDAD VEHICULAR Y PEATONAL EN LAS CALLES MOISES FLORES, ANDRES RAZURI, ARICA, MARISCAL CASTILLA, AV. FAUSTINO SANCHEZ CARRIÓN Y AV. TUPAC AMARU DEL DISTRITO DE CHINCHA ALTA PROVINCIA DE CHINCHA DEPARTAMENTO DE ICA</t>
+        </is>
+      </c>
+      <c r="N53" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:03</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>CP SER-SM-1-2026-MPCH-OC-1</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE CHINCHA - CHINCHA ALTA</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>24/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>09/02/2026</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>25/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>SERVICIO: MANTENIMIENTO DEL SERVICIO DE TRANSITABILIDAD VEHICULAR Y PEATONAL EN LAS CALLES MOISES FLORES, ANDRES RAZURI, ARICA, MARISCAL CASTILLA, AV. FAUSTINO SANCHEZ CARRIÓN Y AV. TUPAC AMARU DEL DISTRITO DE CHINCHA ALTA PROVINCIA DE CHINCHA DEPARTAMENTO DE ICA</t>
+        </is>
+      </c>
+      <c r="N54" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>26/01/2026 15:03</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>CP SER-SM-1-2026-MPCH-OC-1</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD PROVINCIAL DE CHINCHA - CHINCHA ALTA</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>24/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>09/02/2026</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>25/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>SERVICIO: MANTENIMIENTO DEL SERVICIO DE TRANSITABILIDAD VEHICULAR Y PEATONAL EN LAS CALLES MOISES FLORES, ANDRES RAZURI, ARICA, MARISCAL CASTILLA, AV. FAUSTINO SANCHEZ CARRIÓN Y AV. TUPAC AMARU DEL DISTRITO DE CHINCHA ALTA PROVINCIA DE CHINCHA DEPARTAMENTO DE ICA</t>
+        </is>
+      </c>
+      <c r="N55" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>26/01/2026 13:00</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>CP-ABR-6-2026-ESSALUD/RATU-2</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>SEGURO SOCIAL DE SALUD</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr">
+        <is>
           <t>CONTRATACIÓN DEL SERVICIO DE TRASLADO DE PACIENTES REFERIDOS TUMBES-LIMA Y VICEVERSA DE LA RED ASISTENCIAL TUMBES, POR EL PERIODO DE 24 MESES.</t>
         </is>
       </c>
-      <c r="N8" s="2" t="inlineStr">
+      <c r="N56" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>26/01/2026 13:00</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>CP-ABR-6-2026-ESSALUD/RATU-2</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>SEGURO SOCIAL DE SALUD</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE TRASLADO DE PACIENTES REFERIDOS TUMBES-LIMA Y VICEVERSA DE LA RED ASISTENCIAL TUMBES, POR EL PERIODO DE 24 MESES.</t>
+        </is>
+      </c>
+      <c r="N57" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>26/01/2026 13:00</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>CP-ABR-6-2026-ESSALUD/RATU-2</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>SEGURO SOCIAL DE SALUD</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE TRASLADO DE PACIENTES REFERIDOS TUMBES-LIMA Y VICEVERSA DE LA RED ASISTENCIAL TUMBES, POR EL PERIODO DE 24 MESES.</t>
+        </is>
+      </c>
+      <c r="N58" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>26/01/2026 13:00</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>CP-ABR-6-2026-ESSALUD/RATU-2</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>SEGURO SOCIAL DE SALUD</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE TRASLADO DE PACIENTES REFERIDOS TUMBES-LIMA Y VICEVERSA DE LA RED ASISTENCIAL TUMBES, POR EL PERIODO DE 24 MESES.</t>
+        </is>
+      </c>
+      <c r="N59" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>26/01/2026 13:00</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>CP-ABR-6-2026-ESSALUD/RATU-2</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>SEGURO SOCIAL DE SALUD</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE TRASLADO DE PACIENTES REFERIDOS TUMBES-LIMA Y VICEVERSA DE LA RED ASISTENCIAL TUMBES, POR EL PERIODO DE 24 MESES.</t>
+        </is>
+      </c>
+      <c r="N60" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>26/01/2026 13:00</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>CP-ABR-6-2026-ESSALUD/RATU-2</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>SEGURO SOCIAL DE SALUD</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE TRASLADO DE PACIENTES REFERIDOS TUMBES-LIMA Y VICEVERSA DE LA RED ASISTENCIAL TUMBES, POR EL PERIODO DE 24 MESES.</t>
+        </is>
+      </c>
+      <c r="N61" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>26/01/2026 13:00</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>CP-ABR-6-2026-ESSALUD/RATU-2</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>SEGURO SOCIAL DE SALUD</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE TRASLADO DE PACIENTES REFERIDOS TUMBES-LIMA Y VICEVERSA DE LA RED ASISTENCIAL TUMBES, POR EL PERIODO DE 24 MESES.</t>
+        </is>
+      </c>
+      <c r="N62" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>26/01/2026 13:00</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>CP-ABR-6-2026-ESSALUD/RATU-2</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>SEGURO SOCIAL DE SALUD</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE TRASLADO DE PACIENTES REFERIDOS TUMBES-LIMA Y VICEVERSA DE LA RED ASISTENCIAL TUMBES, POR EL PERIODO DE 24 MESES.</t>
+        </is>
+      </c>
+      <c r="N63" s="2" t="inlineStr">
+        <is>
+          <t>Ver Documento</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>26/01/2026 23:28:57</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>26/01/2026 13:00</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>CP-ABR-6-2026-ESSALUD/RATU-2</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>SEGURO SOCIAL DE SALUD</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>03/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>29/01/2026 23:59</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>04/02/2026 23:59</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>CONTRATACIÓN DEL SERVICIO DE TRASLADO DE PACIENTES REFERIDOS TUMBES-LIMA Y VICEVERSA DE LA RED ASISTENCIAL TUMBES, POR EL PERIODO DE 24 MESES.</t>
+        </is>
+      </c>
+      <c r="N64" s="2" t="inlineStr">
         <is>
           <t>Ver Documento</t>
         </is>
@@ -971,6 +4443,62 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N6" r:id="rId5"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N7" r:id="rId6"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N8" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N9" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N10" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N11" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N12" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N13" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N14" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N15" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N16" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N17" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N18" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N19" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N20" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N21" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N22" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N23" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N24" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N25" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N26" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N27" r:id="rId26"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N28" r:id="rId27"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N29" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N30" r:id="rId29"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N31" r:id="rId30"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N32" r:id="rId31"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N33" r:id="rId32"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N34" r:id="rId33"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N35" r:id="rId34"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N36" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N37" r:id="rId36"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N38" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N39" r:id="rId38"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N40" r:id="rId39"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N41" r:id="rId40"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N42" r:id="rId41"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N43" r:id="rId42"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N44" r:id="rId43"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N45" r:id="rId44"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N46" r:id="rId45"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N47" r:id="rId46"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N48" r:id="rId47"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N49" r:id="rId48"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N50" r:id="rId49"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N51" r:id="rId50"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N52" r:id="rId51"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N53" r:id="rId52"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N54" r:id="rId53"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N55" r:id="rId54"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N56" r:id="rId55"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N57" r:id="rId56"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N58" r:id="rId57"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N59" r:id="rId58"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N60" r:id="rId59"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N61" r:id="rId60"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N62" r:id="rId61"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N63" r:id="rId62"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N64" r:id="rId63"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>